<commit_message>
Bug is no more
</commit_message>
<xml_diff>
--- a/Pomiary.xlsx
+++ b/Pomiary.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub\Desktop\Studia\Semestr 4\NiDUC\Symulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988ED06E-F670-4ACA-A307-5DCB6433F29B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308CA7A0-975C-4BB0-A5DB-99C37A0318AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8436" yWindow="612" windowWidth="14112" windowHeight="11364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSCandParityBit" sheetId="1" r:id="rId1"/>
+    <sheet name="BurstErrorandParityBit" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Bit error rate [%]</t>
   </si>
@@ -413,15 +414,10 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H19" sqref="H19:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.21875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -442,16 +438,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>8.0833333333333321</v>
+        <v>8.4166666666666661</v>
       </c>
       <c r="B2">
         <v>7.6923076923076872</v>
       </c>
       <c r="C2">
-        <v>78.302325581395351</v>
+        <v>81.359550561797761</v>
       </c>
       <c r="D2">
-        <v>1.0030508041381839E-2</v>
+        <v>1.09708309173584E-2</v>
       </c>
       <c r="E2">
         <v>0.1</v>
@@ -459,16 +455,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>9.4166666666666661</v>
+        <v>10.08333333333333</v>
       </c>
       <c r="B3">
         <v>7.6923076923076872</v>
       </c>
       <c r="C3">
-        <v>76.692307692307693</v>
+        <v>78.302325581395351</v>
       </c>
       <c r="D3">
-        <v>9.9732875823974609E-3</v>
+        <v>8.9390277862548828E-3</v>
       </c>
       <c r="E3">
         <v>0.1</v>
@@ -476,16 +472,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>9.5833333333333339</v>
+        <v>7.8333333333333339</v>
       </c>
       <c r="B4">
         <v>7.6923076923076872</v>
       </c>
       <c r="C4">
-        <v>75.58682634730539</v>
+        <v>67.701298701298697</v>
       </c>
       <c r="D4">
-        <v>8.9590549468994141E-3</v>
+        <v>9.9732875823974609E-3</v>
       </c>
       <c r="E4">
         <v>0.1</v>
@@ -493,16 +489,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>9.6666666666666661</v>
+        <v>9.9166666666666661</v>
       </c>
       <c r="B5">
         <v>7.6923076923076872</v>
       </c>
       <c r="C5">
-        <v>74.454545454545453</v>
+        <v>75.58682634730539</v>
       </c>
       <c r="D5">
-        <v>9.9761486053466797E-3</v>
+        <v>9.9740028381347656E-3</v>
       </c>
       <c r="E5">
         <v>0.1</v>
@@ -510,16 +506,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>9</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="B6">
         <v>7.6923076923076872</v>
       </c>
       <c r="C6">
-        <v>74.454545454545453</v>
+        <v>68.354838709677409</v>
       </c>
       <c r="D6">
-        <v>9.9763870239257813E-3</v>
+        <v>1.09705924987793E-2</v>
       </c>
       <c r="E6">
         <v>0.1</v>
@@ -527,16 +523,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>10.16666666666667</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>7.6923076923076872</v>
       </c>
       <c r="C7">
-        <v>74.454545454545453</v>
+        <v>70.886792452830193</v>
       </c>
       <c r="D7">
-        <v>1.499557495117188E-2</v>
+        <v>9.9740028381347656E-3</v>
       </c>
       <c r="E7">
         <v>0.1</v>
@@ -544,16 +540,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>9.5833333333333339</v>
+        <v>8.75</v>
       </c>
       <c r="B8">
         <v>7.6923076923076872</v>
       </c>
       <c r="C8">
-        <v>70.886792452830193</v>
+        <v>80.864406779661024</v>
       </c>
       <c r="D8">
-        <v>8.97979736328125E-3</v>
+        <v>9.9732875823974609E-3</v>
       </c>
       <c r="E8">
         <v>0.1</v>
@@ -561,16 +557,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8.75</v>
+        <v>11.75</v>
       </c>
       <c r="B9">
         <v>7.6923076923076872</v>
       </c>
       <c r="C9">
-        <v>76.692307692307693</v>
+        <v>77.771929824561411</v>
       </c>
       <c r="D9">
-        <v>1.1008501052856451E-2</v>
+        <v>9.9756717681884766E-3</v>
       </c>
       <c r="E9">
         <v>0.1</v>
@@ -578,16 +574,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8.9166666666666679</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="B10">
         <v>7.6923076923076872</v>
       </c>
       <c r="C10">
-        <v>77.235294117647058</v>
+        <v>69.636942675159233</v>
       </c>
       <c r="D10">
-        <v>9.9759101867675781E-3</v>
+        <v>9.9732875823974609E-3</v>
       </c>
       <c r="E10">
         <v>0.1</v>
@@ -595,16 +591,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10.16666666666667</v>
+        <v>11.08333333333333</v>
       </c>
       <c r="B11">
         <v>7.6923076923076872</v>
       </c>
       <c r="C11">
-        <v>83.285714285714292</v>
+        <v>75.58682634730539</v>
       </c>
       <c r="D11">
-        <v>9.9759101867675781E-3</v>
+        <v>9.9740028381347656E-3</v>
       </c>
       <c r="E11">
         <v>0.1</v>
@@ -612,16 +608,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>8</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="B12">
         <v>7.6923076923076872</v>
       </c>
       <c r="C12">
-        <v>74.454545454545453</v>
+        <v>73.878048780487802</v>
       </c>
       <c r="D12">
-        <v>9.4530582427978516E-3</v>
+        <v>1.001286506652832E-2</v>
       </c>
       <c r="E12">
         <v>0.1</v>
@@ -629,16 +625,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>9.0833333333333339</v>
+        <v>9.5</v>
       </c>
       <c r="B13">
         <v>7.6923076923076872</v>
       </c>
       <c r="C13">
-        <v>77.771929824561411</v>
+        <v>70.265822784810126</v>
       </c>
       <c r="D13">
-        <v>9.0334415435791016E-3</v>
+        <v>9.9744796752929688E-3</v>
       </c>
       <c r="E13">
         <v>0.1</v>
@@ -646,16 +642,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>8.5</v>
+        <v>9.5833333333333339</v>
       </c>
       <c r="B14">
         <v>7.6923076923076872</v>
       </c>
       <c r="C14">
-        <v>76.692307692307693</v>
+        <v>69</v>
       </c>
       <c r="D14">
-        <v>1.895236968994141E-2</v>
+        <v>1.0935306549072271E-2</v>
       </c>
       <c r="E14">
         <v>0.1</v>
@@ -663,16 +659,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>10.58333333333333</v>
+        <v>8.75</v>
       </c>
       <c r="B15">
         <v>7.6923076923076872</v>
       </c>
       <c r="C15">
-        <v>79.344827586206904</v>
+        <v>78.826589595375722</v>
       </c>
       <c r="D15">
-        <v>1.196575164794922E-2</v>
+        <v>1.1969089508056641E-2</v>
       </c>
       <c r="E15">
         <v>0.1</v>
@@ -680,16 +676,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>9.75</v>
+        <v>8.5</v>
       </c>
       <c r="B16">
         <v>7.6923076923076872</v>
       </c>
       <c r="C16">
-        <v>69.636942675159233</v>
+        <v>77.235294117647058</v>
       </c>
       <c r="D16">
-        <v>1.2003421783447271E-2</v>
+        <v>1.292872428894043E-2</v>
       </c>
       <c r="E16">
         <v>0.1</v>
@@ -706,7 +702,7 @@
         <v>75.024096385542165</v>
       </c>
       <c r="D17">
-        <v>9.9420547485351563E-3</v>
+        <v>1.100277900695801E-2</v>
       </c>
       <c r="E17">
         <v>0.1</v>
@@ -714,16 +710,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>8.5833333333333339</v>
+        <v>9.9166666666666661</v>
       </c>
       <c r="B18">
         <v>7.6923076923076872</v>
       </c>
       <c r="C18">
-        <v>77.235294117647058</v>
+        <v>80.36363636363636</v>
       </c>
       <c r="D18">
-        <v>1.093006134033203E-2</v>
+        <v>1.296520233154297E-2</v>
       </c>
       <c r="E18">
         <v>0.1</v>
@@ -731,16 +727,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>10.33333333333333</v>
+        <v>9.5</v>
       </c>
       <c r="B19">
         <v>7.6923076923076872</v>
       </c>
       <c r="C19">
-        <v>81.849162011173178</v>
+        <v>80.864406779661024</v>
       </c>
       <c r="D19">
-        <v>1.197099685668945E-2</v>
+        <v>1.096820831298828E-2</v>
       </c>
       <c r="E19">
         <v>0.1</v>
@@ -748,16 +744,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
       <c r="B20">
         <v>7.6923076923076872</v>
       </c>
       <c r="C20">
-        <v>80.36363636363636</v>
+        <v>81.359550561797761</v>
       </c>
       <c r="D20">
-        <v>9.9732875823974609E-3</v>
+        <v>8.9402198791503906E-3</v>
       </c>
       <c r="E20">
         <v>0.1</v>
@@ -765,16 +761,388 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>8.6666666666666679</v>
+        <v>10.75</v>
       </c>
       <c r="B21">
         <v>7.6923076923076872</v>
       </c>
       <c r="C21">
-        <v>70.265822784810126</v>
+        <v>79.857142857142861</v>
       </c>
       <c r="D21">
-        <v>9.9384784698486328E-3</v>
+        <v>8.9786052703857422E-3</v>
+      </c>
+      <c r="E21">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>28.666666666666671</v>
+      </c>
+      <c r="B2">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C2">
+        <v>46.165354330708659</v>
+      </c>
+      <c r="D2">
+        <v>1.093339920043945E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>28.583333333333329</v>
+      </c>
+      <c r="B3">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C3">
+        <v>27.18181818181818</v>
+      </c>
+      <c r="D3">
+        <v>9.9351406097412109E-3</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C4">
+        <v>35.666666666666657</v>
+      </c>
+      <c r="D4">
+        <v>1.1933803558349609E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>26.083333333333329</v>
+      </c>
+      <c r="B5">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C5">
+        <v>34.517241379310349</v>
+      </c>
+      <c r="D5">
+        <v>1.2968063354492189E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>25.416666666666661</v>
+      </c>
+      <c r="B6">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C6">
+        <v>33.347826086956523</v>
+      </c>
+      <c r="D6">
+        <v>1.2964487075805661E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>27.833333333333329</v>
+      </c>
+      <c r="B7">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C7">
+        <v>43.193548387096783</v>
+      </c>
+      <c r="D7">
+        <v>1.492738723754883E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>28.083333333333329</v>
+      </c>
+      <c r="B8">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C8">
+        <v>43.193548387096783</v>
+      </c>
+      <c r="D8">
+        <v>1.59611701965332E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>29.333333333333329</v>
+      </c>
+      <c r="B9">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C9">
+        <v>33.347826086956523</v>
+      </c>
+      <c r="D9">
+        <v>1.2964487075805661E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>27.333333333333329</v>
+      </c>
+      <c r="B10">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C10">
+        <v>30.946902654867259</v>
+      </c>
+      <c r="D10">
+        <v>1.196408271789551E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>25.833333333333339</v>
+      </c>
+      <c r="B11">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C11">
+        <v>43.193548387096783</v>
+      </c>
+      <c r="D11">
+        <v>1.296567916870117E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>28.333333333333329</v>
+      </c>
+      <c r="B12">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C12">
+        <v>29.714285714285712</v>
+      </c>
+      <c r="D12">
+        <v>1.001071929931641E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>29.166666666666671</v>
+      </c>
+      <c r="B13">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C13">
+        <v>32.15789473684211</v>
+      </c>
+      <c r="D13">
+        <v>1.096343994140625E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>25.166666666666661</v>
+      </c>
+      <c r="B14">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C14">
+        <v>34.517241379310349</v>
+      </c>
+      <c r="D14">
+        <v>1.097011566162109E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>29.333333333333329</v>
+      </c>
+      <c r="B15">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C15">
+        <v>28.45945945945946</v>
+      </c>
+      <c r="D15">
+        <v>1.1969804763793951E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>26.916666666666671</v>
+      </c>
+      <c r="B16">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C16">
+        <v>46.165354330708659</v>
+      </c>
+      <c r="D16">
+        <v>1.2006044387817379E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>28.583333333333329</v>
+      </c>
+      <c r="B17">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C17">
+        <v>40.074380165289263</v>
+      </c>
+      <c r="D17">
+        <v>1.395845413208008E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C18">
+        <v>39</v>
+      </c>
+      <c r="D18">
+        <v>1.3925790786743161E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>27.583333333333329</v>
+      </c>
+      <c r="B19">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C19">
+        <v>40.074380165289263</v>
+      </c>
+      <c r="D19">
+        <v>1.2964010238647459E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>30.75</v>
+      </c>
+      <c r="B20">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C20">
+        <v>42.170731707317067</v>
+      </c>
+      <c r="D20">
+        <v>1.39620304107666E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>27.333333333333329</v>
+      </c>
+      <c r="B21">
+        <v>7.6923076923076872</v>
+      </c>
+      <c r="C21">
+        <v>25.88073394495413</v>
+      </c>
+      <c r="D21">
+        <v>1.196765899658203E-2</v>
       </c>
       <c r="E21">
         <v>0.1</v>

</xml_diff>